<commit_message>
Export competency matrix to excel done
</commit_message>
<xml_diff>
--- a/ComponentsCollection.xlsx
+++ b/ComponentsCollection.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Код н/д</t>
   </si>
@@ -31,55 +31,76 @@
     <t>Обов'язкові компоненти ОП</t>
   </si>
   <si>
-    <t>ОК 4</t>
-  </si>
-  <si>
-    <t>fавіаdafsaf</t>
+    <t>ОК 1.</t>
+  </si>
+  <si>
+    <t>fавіаdaвіаfsaf</t>
   </si>
   <si>
     <t>залік</t>
   </si>
   <si>
-    <t>ОК 5</t>
-  </si>
-  <si>
-    <t>fавіаdaвіаfsaf</t>
+    <t>ОК 2.</t>
+  </si>
+  <si>
+    <t>ОК 3.</t>
+  </si>
+  <si>
+    <t>ОК 4.</t>
+  </si>
+  <si>
+    <t>ОК 5.</t>
+  </si>
+  <si>
+    <t>ОК 6.</t>
+  </si>
+  <si>
+    <t>ОК 7.</t>
+  </si>
+  <si>
+    <t>ОК 8.</t>
+  </si>
+  <si>
+    <t>ОК 9.</t>
+  </si>
+  <si>
+    <t>ОК 10.</t>
   </si>
   <si>
     <t xml:space="preserve">Загальний обсяг обов'язкових компонент: </t>
   </si>
   <si>
-    <t>30 кредитів</t>
-  </si>
-  <si>
-    <t>ВБ 1</t>
-  </si>
-  <si>
-    <t>фаввфіа</t>
-  </si>
-  <si>
-    <t>ВБ 2</t>
-  </si>
-  <si>
-    <t>fdsaf</t>
-  </si>
-  <si>
-    <t>ВБ 3</t>
-  </si>
-  <si>
-    <t>fdafsaf</t>
+    <t>180 кредитів</t>
+  </si>
+  <si>
+    <t>ВБ 1.</t>
+  </si>
+  <si>
+    <t>ВБ 2.</t>
+  </si>
+  <si>
+    <t>ВБ 3.</t>
+  </si>
+  <si>
+    <t>ВБ 4.</t>
+  </si>
+  <si>
+    <t>ВБ 5.</t>
+  </si>
+  <si>
+    <t>ВБ 6.</t>
   </si>
   <si>
     <t xml:space="preserve">Загальний обсяг вибіркових компонент: </t>
   </si>
   <si>
-    <t>45 кредитів</t>
+    <t>60 кредитів</t>
   </si>
   <si>
     <t xml:space="preserve">ЗАГАЛЬНИЙ ОБСЯГ ОСВІТНЬОЇ ПРОГРАМИ: </t>
   </si>
   <si>
-    <t>75 кредитів</t>
+    <t>240 кредитів</t>
   </si>
 </sst>
 </file>
@@ -96,14 +117,14 @@
     <font>
       <sz val="12"/>
       <color/>
-      <name val="Calibri"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
     </font>
     <font>
       <b val="1"/>
       <sz val="12"/>
       <color/>
-      <name val="Calibri"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -479,7 +500,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -490,34 +511,38 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -525,13 +550,13 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -539,47 +564,197 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3" t="s">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
   </mergeCells>
 </worksheet>
 </file>
</xml_diff>